<commit_message>
added files and scripts and updated summary
</commit_message>
<xml_diff>
--- a/Summary of Knowledge Databases.xlsx
+++ b/Summary of Knowledge Databases.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38220" yWindow="2840" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="51940" yWindow="5980" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="90">
   <si>
     <t>Knowledge Bases</t>
   </si>
@@ -272,9 +273,6 @@
     <t>not sure</t>
   </si>
   <si>
-    <t>not</t>
-  </si>
-  <si>
     <t>in progress,  writing script to automate</t>
   </si>
   <si>
@@ -282,13 +280,31 @@
   </si>
   <si>
     <t>need script to get pmid</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Updated in tool</t>
+  </si>
+  <si>
+    <t>Last Updated in DB</t>
+  </si>
+  <si>
+    <t>Monthly?</t>
+  </si>
+  <si>
+    <t>Unsure  if it still updated</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +357,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -363,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -391,6 +413,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -671,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,7 +870,7 @@
       <c r="H7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="19" t="s">
         <v>76</v>
       </c>
       <c r="J7" s="14" t="s">
@@ -895,11 +926,11 @@
       <c r="H8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="15" t="s">
-        <v>82</v>
+      <c r="J8" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15" t="str">
@@ -951,10 +982,12 @@
       <c r="H9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="15"/>
+      <c r="I9" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="K9" s="15"/>
       <c r="L9" s="16" t="str">
         <f>HYPERLINK("https://www.ncbi.nlm.nih.gov/pubmed/27684579","27684579")</f>
@@ -1005,11 +1038,11 @@
       <c r="H10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="17" t="s">
-        <v>82</v>
+      <c r="J10" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="K10" s="17"/>
       <c r="L10" s="18" t="str">
@@ -1061,11 +1094,11 @@
       <c r="H11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="20" t="s">
         <v>80</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="15" t="str">
@@ -1117,11 +1150,11 @@
       <c r="H12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="20" t="s">
         <v>78</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" s="14"/>
       <c r="L12" s="14" t="s">
@@ -1173,10 +1206,10 @@
         <v>24</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14" t="s">
@@ -1231,7 +1264,7 @@
         <v>78</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="16" t="str">
@@ -1600,4 +1633,394 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
+    <col min="3" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="24">
+        <v>43018</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="25">
+        <v>43018</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F10" r:id="rId3"/>
+    <hyperlink ref="F11" r:id="rId4"/>
+    <hyperlink ref="F12" r:id="rId5" location="/"/>
+    <hyperlink ref="F13" r:id="rId6" location="/home"/>
+    <hyperlink ref="F14" r:id="rId7"/>
+    <hyperlink ref="A19" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added some files, with updated jax files and notes from manual clean
</commit_message>
<xml_diff>
--- a/Summary of Knowledge Databases.xlsx
+++ b/Summary of Knowledge Databases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51940" yWindow="5980" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="38880" yWindow="4000" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="93">
   <si>
     <t>Knowledge Bases</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>Done,  But going to write script to automate</t>
+  </si>
+  <si>
+    <t>not updated anymore</t>
+  </si>
+  <si>
+    <t>schema changed for genes table and needs to be updated</t>
   </si>
 </sst>
 </file>
@@ -385,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -422,6 +431,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -702,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1053,7 @@
         <v>79</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="K10" s="17"/>
       <c r="L10" s="18" t="str">
@@ -1640,7 +1651,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1737,10 +1748,12 @@
       <c r="C8" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="21"/>
+      <c r="D8" s="25">
+        <v>43025</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="F8" s="15" t="s">
         <v>34</v>
       </c>
@@ -1777,10 +1790,12 @@
       <c r="C10" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="22"/>
+      <c r="D10" s="26">
+        <v>43028</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>65</v>
+      </c>
       <c r="F10" s="15" t="s">
         <v>43</v>
       </c>
@@ -1796,9 +1811,7 @@
       <c r="C11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="20"/>
       <c r="F11" s="15" t="s">
         <v>46</v>
@@ -1815,10 +1828,12 @@
       <c r="C12" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="20"/>
+      <c r="D12" s="27">
+        <v>43025</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="F12" s="15" t="s">
         <v>49</v>
       </c>
@@ -1867,7 +1882,9 @@
       <c r="B15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15" t="s">
@@ -1882,7 +1899,9 @@
       <c r="B16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="15" t="s">

</xml_diff>

<commit_message>
reorganized files and updates summary
</commit_message>
<xml_diff>
--- a/Summary of Knowledge Databases.xlsx
+++ b/Summary of Knowledge Databases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38880" yWindow="4000" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="37300" yWindow="4320" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -297,9 +297,6 @@
     <t>Unsure  if it still updated</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Done,  But going to write script to automate</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>schema changed for genes table and needs to be updated</t>
+  </si>
+  <si>
+    <t>is ready, but not yet uploaded</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1053,7 @@
         <v>79</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K10" s="17"/>
       <c r="L10" s="18" t="str">
@@ -1650,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1752,7 +1752,7 @@
         <v>43025</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>34</v>
@@ -1867,7 +1867,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="15" t="s">
@@ -1883,7 +1883,7 @@
         <v>64</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -1900,7 +1900,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>

</xml_diff>